<commit_message>
Fitur Multi Size & Gambar Detail
</commit_message>
<xml_diff>
--- a/database/FileExcel/Atribut.xlsx
+++ b/database/FileExcel/Atribut.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yovie\persediaanapp-magang\database\FileExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E446A2-E191-451F-8407-845233B6C50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FEC056D-621A-4BEE-8043-80605C1275F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8130" yWindow="600" windowWidth="6670" windowHeight="10080" xr2:uid="{B1A6D6DA-43F5-4D03-876B-1BE0E6BF7134}"/>
+    <workbookView xWindow="1750" yWindow="410" windowWidth="6670" windowHeight="10080" xr2:uid="{B1A6D6DA-43F5-4D03-876B-1BE0E6BF7134}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,17 +32,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>id_product</t>
-  </si>
-  <si>
-    <t>size</t>
-  </si>
-  <si>
     <t>stock</t>
   </si>
   <si>
@@ -59,6 +53,33 @@
   </si>
   <si>
     <t>XXL</t>
+  </si>
+  <si>
+    <t>TS001-M</t>
+  </si>
+  <si>
+    <t>TS002-L</t>
+  </si>
+  <si>
+    <t>TS001-L</t>
+  </si>
+  <si>
+    <t>TS001-XL</t>
+  </si>
+  <si>
+    <t>TS002-M</t>
+  </si>
+  <si>
+    <t>TS002-XXL</t>
+  </si>
+  <si>
+    <t>id_barang</t>
+  </si>
+  <si>
+    <t>ukuran</t>
+  </si>
+  <si>
+    <t>sku</t>
   </si>
 </sst>
 </file>
@@ -416,51 +437,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC210C0-9D73-46BA-9C56-AD0FD5D86CE8}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
       <c r="D2">
         <v>12</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="J2" s="1"/>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
       <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>2</v>
       </c>
@@ -468,16 +495,19 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>12</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>3</v>
       </c>
@@ -485,16 +515,19 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>12</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>4</v>
       </c>
@@ -502,16 +535,19 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>10</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>5</v>
       </c>
@@ -519,16 +555,19 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>6</v>
       </c>
@@ -536,12 +575,15 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>10</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
edit route slug di Admin
</commit_message>
<xml_diff>
--- a/database/FileExcel/Atribut.xlsx
+++ b/database/FileExcel/Atribut.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yovie\persediaanapp-magang\database\FileExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A505E2F0-0799-4150-A09F-C47F04CCAA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A394B4BE-9361-47AD-B37C-5E7F157DBD5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7450" yWindow="440" windowWidth="11440" windowHeight="9330" xr2:uid="{B1A6D6DA-43F5-4D03-876B-1BE0E6BF7134}"/>
+    <workbookView xWindow="6570" yWindow="2990" windowWidth="11440" windowHeight="7810" xr2:uid="{B1A6D6DA-43F5-4D03-876B-1BE0E6BF7134}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,22 +64,22 @@
     <t>TS002-M</t>
   </si>
   <si>
+    <t>ukuran</t>
+  </si>
+  <si>
+    <t>sku</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>TS001-S</t>
+  </si>
+  <si>
+    <t>TS002-XL</t>
+  </si>
+  <si>
     <t>id_barang</t>
-  </si>
-  <si>
-    <t>ukuran</t>
-  </si>
-  <si>
-    <t>sku</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>TS001-S</t>
-  </si>
-  <si>
-    <t>TS002-XL</t>
   </si>
 </sst>
 </file>
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC210C0-9D73-46BA-9C56-AD0FD5D86CE8}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -450,16 +450,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -473,13 +473,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2">
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -581,7 +581,7 @@
         <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -589,5 +589,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>